<commit_message>
Creada la clase de serialización de sistemas lineales y corregidos los nombres de métodos de inicialización y obtenición de objetos como arrays.
</commit_message>
<xml_diff>
--- a/practica2/trunk/TDAs/doc/metricas/metricas_sel.xlsx
+++ b/practica2/trunk/TDAs/doc/metricas/metricas_sel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Refactorización general</t>
+  </si>
+  <si>
+    <t>Código para lectura/escritura del SEL</t>
   </si>
 </sst>
 </file>
@@ -1111,10 +1114,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>7.441860465116272E-2</c:v>
+                  <c:v>6.2256809338521346E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.92558139534883732</c:v>
+                  <c:v>0.93774319066147871</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1702,7 +1705,7 @@
   <dimension ref="A1:IU50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2211,21 +2214,37 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
+      <c r="A18" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="22">
+        <v>70</v>
+      </c>
+      <c r="C18" s="22">
+        <v>86</v>
+      </c>
+      <c r="D18" s="23">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E18" s="23">
+        <v>0.1875</v>
+      </c>
+      <c r="F18" s="23">
+        <v>0.21666666666666667</v>
+      </c>
       <c r="G18" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="23"/>
+        <v>2.9166666666666674E-2</v>
+      </c>
+      <c r="H18" s="22">
+        <v>0</v>
+      </c>
+      <c r="I18" s="23">
+        <v>0</v>
+      </c>
       <c r="J18" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.9166666666666674E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -2324,21 +2343,21 @@
       </c>
       <c r="B24" s="24">
         <f>SUM(B6:B23)</f>
-        <v>267</v>
+        <v>337</v>
       </c>
       <c r="C24" s="24">
         <f>SUM(C6:C23)</f>
-        <v>239</v>
+        <v>325</v>
       </c>
       <c r="D24" s="25">
         <f>SUM(D6:D23)</f>
-        <v>0.12083333333333333</v>
+        <v>0.13472222222222222</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="25">
         <f>SUM(G6:G23)</f>
-        <v>0.13819444444444459</v>
+        <v>0.16736111111111127</v>
       </c>
       <c r="H24" s="26">
         <f>SUM(H6:H23)</f>
@@ -2350,7 +2369,7 @@
       </c>
       <c r="J24" s="28">
         <f>SUM(J6:J23)</f>
-        <v>0.14930555555555569</v>
+        <v>0.17847222222222237</v>
       </c>
       <c r="K24" s="4"/>
     </row>
@@ -2360,7 +2379,7 @@
       </c>
       <c r="B25" s="20">
         <f>IF(EXACT($C$24, 0),"-",ABS($B$24-$C$24)/$C$24)</f>
-        <v>0.11715481171548117</v>
+        <v>3.6923076923076927E-2</v>
       </c>
       <c r="D25" s="5"/>
       <c r="J25" s="3"/>
@@ -2378,7 +2397,7 @@
       </c>
       <c r="B28" s="32">
         <f>C24</f>
-        <v>239</v>
+        <v>325</v>
       </c>
       <c r="C28" s="9"/>
     </row>
@@ -2388,7 +2407,7 @@
       </c>
       <c r="B29" s="34">
         <f>IF(EXACT($B$28,0),"-",$B$28/((J24-INT(J24))*24))</f>
-        <v>66.697674418604592</v>
+        <v>75.875486381322901</v>
       </c>
       <c r="C29" s="9"/>
     </row>
@@ -2398,7 +2417,7 @@
       </c>
       <c r="B30" s="34">
         <f>IF(EXACT($B$28,0),"-",H24/($B$28/10))</f>
-        <v>8.3682008368200847E-2</v>
+        <v>6.1538461538461542E-2</v>
       </c>
       <c r="C30" s="9"/>
     </row>
@@ -2408,7 +2427,7 @@
       </c>
       <c r="B31" s="36">
         <f>IF(EXACT($B$28,0),"-",H24/$B$28)</f>
-        <v>8.368200836820083E-3</v>
+        <v>6.1538461538461538E-3</v>
       </c>
       <c r="C31" s="44" t="s">
         <v>19</v>
@@ -2424,7 +2443,7 @@
       </c>
       <c r="C32" s="40">
         <f>IF(EXACT(J24,0),5%,B32/J24)</f>
-        <v>7.441860465116272E-2</v>
+        <v>6.2256809338521346E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2433,11 +2452,11 @@
       </c>
       <c r="B33" s="39">
         <f>G24</f>
-        <v>0.13819444444444459</v>
+        <v>0.16736111111111127</v>
       </c>
       <c r="C33" s="41">
         <f>IF(EXACT(J24,0),95%,B33/J24)</f>
-        <v>0.92558139534883732</v>
+        <v>0.93774319066147871</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2446,7 +2465,7 @@
       </c>
       <c r="B34" s="39">
         <f>C2+C3+J24</f>
-        <v>0.16527777777777786</v>
+        <v>0.19444444444444453</v>
       </c>
       <c r="D34" s="6"/>
     </row>

</xml_diff>